<commit_message>
Added DirectionalLight and rotation
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -910,27 +910,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="101.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" customWidth="1"/>
-    <col min="8" max="9" width="25.81640625" customWidth="1"/>
-    <col min="10" max="10" width="24.7265625" customWidth="1"/>
-    <col min="11" max="11" width="24.54296875" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -984,7 +984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>66</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="H4" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1051,14 +1051,14 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>65</v>
       </c>
@@ -1074,10 +1074,12 @@
       <c r="E5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1093,7 +1095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -1114,7 +1116,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1130,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>67</v>
       </c>
@@ -1161,7 +1163,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1182,11 +1184,11 @@
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
@@ -1195,7 +1197,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1226,7 +1228,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>45</v>
       </c>
@@ -1247,7 +1249,7 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
@@ -1260,7 +1262,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -1285,7 +1287,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1302,7 +1304,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1319,7 +1321,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1336,7 +1338,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1353,7 +1355,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1370,7 +1372,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1391,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>48</v>
       </c>
@@ -1405,10 +1407,12 @@
       <c r="E18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1416,7 +1420,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -1441,7 +1445,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -1466,7 +1470,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>36</v>
       </c>
@@ -1491,7 +1495,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
@@ -1516,7 +1520,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>47</v>
       </c>
@@ -1545,7 +1549,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>68</v>
       </c>
@@ -1570,7 +1574,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1587,7 +1591,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1604,7 +1608,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1621,7 +1625,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1638,7 +1642,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
@@ -1657,7 +1661,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>51</v>
       </c>
@@ -1673,10 +1677,12 @@
       <c r="E30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1684,7 +1690,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>52</v>
       </c>
@@ -1711,7 +1717,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
@@ -1738,7 +1744,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>54</v>
       </c>
@@ -1763,7 +1769,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>55</v>
       </c>
@@ -1776,11 +1782,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1788,7 +1798,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>56</v>
       </c>
@@ -1813,7 +1823,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>57</v>
       </c>
@@ -1838,7 +1848,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>58</v>
       </c>
@@ -1863,7 +1873,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>33</v>
       </c>
@@ -1888,7 +1898,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>34</v>
       </c>
@@ -1915,7 +1925,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>69</v>
       </c>
@@ -1940,7 +1950,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1957,7 +1967,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1974,7 +1984,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1991,7 +2001,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2020,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>59</v>
       </c>
@@ -2035,7 +2045,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>70</v>
       </c>
@@ -2060,7 +2070,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>71</v>
       </c>
@@ -2085,7 +2095,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2102,7 +2112,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2119,7 +2129,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2136,7 +2146,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2153,7 +2163,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2170,7 +2180,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>7</v>
       </c>
@@ -2189,7 +2199,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>60</v>
       </c>
@@ -2214,7 +2224,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>72</v>
       </c>
@@ -2239,7 +2249,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>61</v>
       </c>
@@ -2264,7 +2274,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>73</v>
       </c>
@@ -2289,7 +2299,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2306,7 +2316,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2323,7 +2333,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2340,7 +2350,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2357,7 +2367,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2374,7 +2384,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2391,7 +2401,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>6</v>
       </c>
@@ -2410,7 +2420,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>62</v>
       </c>
@@ -2439,7 +2449,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>74</v>
       </c>
@@ -2468,7 +2478,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>75</v>
       </c>
@@ -2493,7 +2503,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>76</v>
       </c>
@@ -2518,7 +2528,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2535,7 +2545,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2552,7 +2562,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2569,7 +2579,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2586,7 +2596,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2603,7 +2613,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2632,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>0</v>
       </c>
@@ -2647,7 +2657,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2664,7 +2674,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2681,7 +2691,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2698,7 +2708,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2715,7 +2725,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2732,7 +2742,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2749,7 +2759,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2766,7 +2776,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2783,7 +2793,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2800,7 +2810,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2817,7 +2827,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="15"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2831,7 +2841,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2845,7 +2855,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -2859,7 +2869,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>39</v>
       </c>
@@ -2883,7 +2893,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>18</v>
       </c>
@@ -2901,7 +2911,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>31</v>
       </c>
@@ -2919,7 +2929,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -2933,7 +2943,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -2947,78 +2957,78 @@
       <c r="K93" s="5"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="16"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="16"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="16"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="17"/>
     </row>
   </sheetData>
@@ -3043,7 +3053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3125,7 +3135,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3137,7 +3147,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Point Light and Moving
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
@@ -1706,10 +1706,12 @@
       <c r="E31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1757,11 +1759,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1811,11 +1817,15 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -3053,7 +3063,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added spotlight and move with camera
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -910,27 +910,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="101.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" customWidth="1"/>
-    <col min="8" max="9" width="25.81640625" customWidth="1"/>
-    <col min="10" max="10" width="24.7265625" customWidth="1"/>
-    <col min="11" max="11" width="24.54296875" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -984,7 +984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>66</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1051,14 +1051,14 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>65</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1132,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>67</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1192,12 +1192,12 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>45</v>
       </c>
@@ -1249,11 +1249,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -1262,7 +1262,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1304,7 +1304,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1321,7 +1321,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1338,7 +1338,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1355,7 +1355,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1372,7 +1372,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>48</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>36</v>
       </c>
@@ -1495,7 +1495,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
@@ -1520,7 +1520,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>47</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>68</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1591,7 +1591,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1608,7 +1608,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1625,7 +1625,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1642,7 +1642,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>51</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>52</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
@@ -1735,10 +1735,12 @@
       <c r="E32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1746,7 +1748,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>54</v>
       </c>
@@ -1775,7 +1777,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>55</v>
       </c>
@@ -1804,7 +1806,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>56</v>
       </c>
@@ -1833,7 +1835,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>57</v>
       </c>
@@ -1849,10 +1851,12 @@
       <c r="E36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -1860,7 +1864,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>58</v>
       </c>
@@ -1885,7 +1889,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>33</v>
       </c>
@@ -1910,7 +1914,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>34</v>
       </c>
@@ -1939,7 +1943,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>69</v>
       </c>
@@ -1964,7 +1968,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1981,7 +1985,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1998,7 +2002,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2015,7 +2019,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2038,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>59</v>
       </c>
@@ -2059,7 +2063,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>70</v>
       </c>
@@ -2084,7 +2088,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>71</v>
       </c>
@@ -2109,7 +2113,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2126,7 +2130,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2143,7 +2147,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2160,7 +2164,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2177,7 +2181,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2194,7 +2198,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>7</v>
       </c>
@@ -2213,7 +2217,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>60</v>
       </c>
@@ -2238,7 +2242,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>72</v>
       </c>
@@ -2263,7 +2267,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>61</v>
       </c>
@@ -2288,7 +2292,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>73</v>
       </c>
@@ -2313,7 +2317,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2330,7 +2334,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2347,7 +2351,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2364,7 +2368,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2381,7 +2385,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2398,7 +2402,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2415,7 +2419,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>6</v>
       </c>
@@ -2434,7 +2438,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>62</v>
       </c>
@@ -2463,7 +2467,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>74</v>
       </c>
@@ -2492,7 +2496,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>75</v>
       </c>
@@ -2517,7 +2521,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>76</v>
       </c>
@@ -2542,7 +2546,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2559,7 +2563,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2576,7 +2580,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2593,7 +2597,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2610,7 +2614,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2627,7 +2631,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>5</v>
       </c>
@@ -2646,7 +2650,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2675,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2688,7 +2692,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2705,7 +2709,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2722,7 +2726,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2739,7 +2743,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2756,7 +2760,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2773,7 +2777,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2790,7 +2794,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2807,7 +2811,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2824,7 +2828,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2841,7 +2845,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="15"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2855,7 +2859,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2869,7 +2873,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -2883,7 +2887,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>39</v>
       </c>
@@ -2907,7 +2911,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>18</v>
       </c>
@@ -2917,7 +2921,9 @@
       <c r="C90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -2927,7 +2933,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>31</v>
       </c>
@@ -2937,7 +2943,9 @@
       <c r="C91" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -2947,7 +2955,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -2961,7 +2969,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -2975,78 +2983,78 @@
       <c r="K93" s="5"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="16"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="16"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="16"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="17"/>
     </row>
   </sheetData>
@@ -3071,7 +3079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3153,7 +3161,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3165,7 +3173,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Specular Map with out specular color
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -911,26 +914,26 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="101.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="101.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
+    <col min="8" max="9" width="25.81640625" customWidth="1"/>
+    <col min="10" max="10" width="24.7265625" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="24.1796875" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
@@ -946,7 +949,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -984,7 +987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>66</v>
       </c>
@@ -1043,7 +1046,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1055,10 +1058,10 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>65</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -1129,10 +1132,10 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>67</v>
       </c>
@@ -1163,7 +1166,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1192,12 +1195,12 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>44</v>
       </c>
@@ -1228,7 +1231,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>45</v>
       </c>
@@ -1253,16 +1256,16 @@
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -1287,7 +1290,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1304,7 +1307,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1321,7 +1324,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1338,7 +1341,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1355,7 +1358,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1372,7 +1375,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1394,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>48</v>
       </c>
@@ -1420,7 +1423,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -1445,7 +1448,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -1470,7 +1473,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>36</v>
       </c>
@@ -1495,7 +1498,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1527,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>47</v>
       </c>
@@ -1553,7 +1556,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>68</v>
       </c>
@@ -1578,7 +1581,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1595,7 +1598,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1612,7 +1615,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1629,7 +1632,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1646,7 +1649,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1668,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>51</v>
       </c>
@@ -1694,7 +1697,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>52</v>
       </c>
@@ -1723,7 +1726,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
@@ -1752,7 +1755,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>54</v>
       </c>
@@ -1781,7 +1784,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>55</v>
       </c>
@@ -1810,7 +1813,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>56</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>57</v>
       </c>
@@ -1868,7 +1871,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>58</v>
       </c>
@@ -1893,7 +1896,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
         <v>33</v>
       </c>
@@ -1918,7 +1921,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>34</v>
       </c>
@@ -1947,7 +1950,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
         <v>69</v>
       </c>
@@ -1960,11 +1963,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -1972,7 +1979,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="11"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1989,7 +1996,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="11"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2006,7 +2013,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="11"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2023,7 +2030,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>8</v>
       </c>
@@ -2042,7 +2049,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
         <v>59</v>
       </c>
@@ -2067,7 +2074,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
         <v>70</v>
       </c>
@@ -2092,7 +2099,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
         <v>71</v>
       </c>
@@ -2117,7 +2124,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="11"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2134,7 +2141,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="11"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2151,7 +2158,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="11"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2168,7 +2175,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="11"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2185,7 +2192,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2202,7 +2209,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
         <v>7</v>
       </c>
@@ -2221,7 +2228,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
         <v>60</v>
       </c>
@@ -2250,7 +2257,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
         <v>72</v>
       </c>
@@ -2263,11 +2270,15 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2275,7 +2286,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>61</v>
       </c>
@@ -2300,7 +2311,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
         <v>73</v>
       </c>
@@ -2325,7 +2336,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="11"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2342,7 +2353,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="11"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2359,7 +2370,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="11"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2376,7 +2387,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="11"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2393,7 +2404,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="11"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2410,7 +2421,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="11"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2427,7 +2438,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>6</v>
       </c>
@@ -2446,7 +2457,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
         <v>62</v>
       </c>
@@ -2475,7 +2486,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
         <v>74</v>
       </c>
@@ -2504,7 +2515,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>75</v>
       </c>
@@ -2529,7 +2540,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>76</v>
       </c>
@@ -2554,7 +2565,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="11"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2571,7 +2582,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="11"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2588,7 +2599,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2605,7 +2616,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="11"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2622,7 +2633,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="11"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2639,7 +2650,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>5</v>
       </c>
@@ -2658,7 +2669,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>0</v>
       </c>
@@ -2683,7 +2694,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="11"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2700,7 +2711,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="11"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2717,7 +2728,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="11"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2734,7 +2745,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="11"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2751,7 +2762,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="11"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2768,7 +2779,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="11"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2785,7 +2796,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="11"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2802,7 +2813,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="11"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2819,7 +2830,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="11"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2836,7 +2847,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="11"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2853,7 +2864,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="15"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2867,7 +2878,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="14"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2881,7 +2892,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="14"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -2895,7 +2906,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>39</v>
       </c>
@@ -2919,7 +2930,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="14" t="s">
         <v>18</v>
       </c>
@@ -2939,7 +2950,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
         <v>31</v>
       </c>
@@ -2959,7 +2970,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="14"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -2973,7 +2984,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="14"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -2987,78 +2998,78 @@
       <c r="K93" s="5"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="16"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="16"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="16"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="16"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="16"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="16"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="16"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="16"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="16"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="16"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="16"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="16"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="16"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="16"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="16"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="16"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="16"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="16"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="16"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="16"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="16"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="16"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="17"/>
     </row>
   </sheetData>
@@ -3083,7 +3094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3165,7 +3176,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3177,7 +3188,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Frustum cull on CPU added
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3098,7 +3098,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Geometry Shader drawing bounding box
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -914,7 +914,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1054,11 +1054,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1136,7 +1136,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1152,11 +1152,15 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1256,15 +1260,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1516,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>76</v>
@@ -1939,14 +1943,14 @@
         <v>3</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>76</v>
       </c>
       <c r="G39" s="8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>

</xml_diff>

<commit_message>
Frustum Culling via CPU done
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -914,7 +914,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1054,11 +1054,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1136,7 +1136,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1260,15 +1260,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2070,11 +2070,15 @@
       <c r="D45" s="5">
         <v>5</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G45" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -2948,7 +2952,9 @@
       <c r="C90" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -2968,7 +2974,9 @@
       <c r="C91" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3102,7 +3110,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
MileStone II turn in
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,11 +1054,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1136,7 +1136,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1260,15 +1260,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1444,11 +1444,15 @@
       <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -3110,7 +3114,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Roughness / Metallic map supported
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1136,7 +1136,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2959,7 +2959,9 @@
       <c r="D90" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -2981,7 +2983,9 @@
       <c r="D91" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3114,7 +3118,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added wave Post Effect
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -916,27 +916,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="101.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="101.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
+    <col min="8" max="9" width="25.81640625" customWidth="1"/>
+    <col min="10" max="10" width="24.7265625" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="24.1796875" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>78</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>79</v>
       </c>
@@ -990,7 +990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>64</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
@@ -1061,10 +1061,10 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>63</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>40</v>
       </c>
@@ -1139,10 +1139,10 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -1211,7 +1211,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>43</v>
       </c>
@@ -1271,12 +1271,12 @@
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>44</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1318,7 +1318,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1335,7 +1335,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1352,7 +1352,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1369,7 +1369,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1386,7 +1386,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>47</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>48</v>
       </c>
@@ -1476,11 +1476,15 @@
       <c r="D20" s="5">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1488,7 +1492,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>34</v>
       </c>
@@ -1513,7 +1517,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>33</v>
       </c>
@@ -1542,7 +1546,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>45</v>
       </c>
@@ -1571,7 +1575,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>66</v>
       </c>
@@ -1596,7 +1600,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1613,7 +1617,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1630,7 +1634,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1647,7 +1651,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1664,7 +1668,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1687,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>49</v>
       </c>
@@ -1712,7 +1716,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>50</v>
       </c>
@@ -1741,7 +1745,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
@@ -1770,7 +1774,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>52</v>
       </c>
@@ -1799,7 +1803,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>53</v>
       </c>
@@ -1828,7 +1832,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>54</v>
       </c>
@@ -1857,7 +1861,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>55</v>
       </c>
@@ -1886,7 +1890,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>56</v>
       </c>
@@ -1911,7 +1915,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
@@ -1936,7 +1940,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>32</v>
       </c>
@@ -1965,7 +1969,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
         <v>67</v>
       </c>
@@ -1994,7 +1998,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="11"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2011,7 +2015,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="11"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2028,7 +2032,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="11"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2045,7 +2049,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>8</v>
       </c>
@@ -2064,7 +2068,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
         <v>57</v>
       </c>
@@ -2093,7 +2097,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
         <v>68</v>
       </c>
@@ -2122,7 +2126,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
         <v>69</v>
       </c>
@@ -2147,7 +2151,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="11"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2164,7 +2168,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="11"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2181,7 +2185,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="11"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2198,7 +2202,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="11"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2215,7 +2219,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2232,7 +2236,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="12" t="s">
         <v>7</v>
       </c>
@@ -2251,7 +2255,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
         <v>58</v>
       </c>
@@ -2280,7 +2284,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
         <v>70</v>
       </c>
@@ -2309,7 +2313,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>59</v>
       </c>
@@ -2334,7 +2338,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
         <v>71</v>
       </c>
@@ -2359,7 +2363,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="11"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2376,7 +2380,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="11"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2393,7 +2397,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="11"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2410,7 +2414,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="11"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2427,7 +2431,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="11"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2444,7 +2448,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="11"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2461,7 +2465,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>6</v>
       </c>
@@ -2480,7 +2484,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
         <v>60</v>
       </c>
@@ -2509,7 +2513,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
         <v>72</v>
       </c>
@@ -2538,7 +2542,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>73</v>
       </c>
@@ -2563,7 +2567,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>74</v>
       </c>
@@ -2588,7 +2592,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="11"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2605,7 +2609,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="11"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2622,7 +2626,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2639,7 +2643,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="11"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2656,7 +2660,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="11"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2673,7 +2677,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>5</v>
       </c>
@@ -2692,7 +2696,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>0</v>
       </c>
@@ -2705,11 +2709,15 @@
       <c r="D75" s="5">
         <v>5</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G75" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -2717,7 +2725,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="11"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2734,7 +2742,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="11"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2751,7 +2759,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="11"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2768,7 +2776,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="11"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2785,7 +2793,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="11"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2802,7 +2810,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="11"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2819,7 +2827,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="11"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2836,7 +2844,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="11"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2853,7 +2861,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="11"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2870,7 +2878,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="11"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2887,7 +2895,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="15"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2901,7 +2909,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="14"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2915,7 +2923,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="14"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -2929,7 +2937,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>37</v>
       </c>
@@ -2953,7 +2961,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="14" t="s">
         <v>18</v>
       </c>
@@ -2977,7 +2985,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="14" t="s">
         <v>29</v>
       </c>
@@ -3001,7 +3009,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="14"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -3015,7 +3023,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="14"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3029,78 +3037,78 @@
       <c r="K93" s="5"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="16"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="16"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="16"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="16"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="16"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="16"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="16"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="16"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="16"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="16"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="16"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="16"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="16"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="16"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="16"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="16"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="16"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="16"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="16"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="16"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="16"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="16"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="17"/>
     </row>
   </sheetData>
@@ -3125,7 +3133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3207,7 +3215,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3219,7 +3227,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>